<commit_message>
save user of excel
</commit_message>
<xml_diff>
--- a/src/usuarios.xlsx
+++ b/src/usuarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB683A2-E608-4339-9ACF-3902F9804F36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE936F9-D82C-44EE-8D49-9D62BC2536FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>name</t>
   </si>
@@ -36,9 +36,6 @@
     <t>email</t>
   </si>
   <si>
-    <t>roles</t>
-  </si>
-  <si>
     <t>Jose</t>
   </si>
   <si>
@@ -51,16 +48,10 @@
     <t>ronal@ronal</t>
   </si>
   <si>
-    <t>admin</t>
-  </si>
-  <si>
     <t>Carlos</t>
   </si>
   <si>
     <t>carlos@carlos</t>
-  </si>
-  <si>
-    <t>user</t>
   </si>
 </sst>
 </file>
@@ -417,15 +408,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -435,49 +426,37 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>11</v>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>